<commit_message>
Updated testng and whereToBuy files
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/whereToBuyTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/whereToBuyTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22185" windowHeight="8970"/>
+    <workbookView windowWidth="22188" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="headerVerification" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>testcase</t>
   </si>
@@ -22,13 +22,19 @@
     <t>execution</t>
   </si>
   <si>
+    <t>expectedUrl</t>
+  </si>
+  <si>
     <t>expectedHeader</t>
   </si>
   <si>
-    <t>Verify 'Where To Buy' header is displayed</t>
+    <t>Verify 'Where To Buy' header</t>
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>where-to-buy</t>
   </si>
   <si>
     <t>Where To Buy</t>
@@ -966,15 +972,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,16 +990,22 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all tests for Where To Buy module
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/whereToBuyTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/whereToBuyTestData.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9024"/>
+    <workbookView windowWidth="22188" windowHeight="9024" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="headerVerification" sheetId="1" r:id="rId1"/>
+    <sheet name="productSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="changeCategorySize" sheetId="3" r:id="rId3"/>
+    <sheet name="verifyStores" sheetId="4" r:id="rId4"/>
+    <sheet name="verifyLocations" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>testcase</t>
   </si>
@@ -31,13 +35,146 @@
     <t>Verify 'Where To Buy' header</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>where-to-buy</t>
   </si>
   <si>
     <t>Where To Buy</t>
+  </si>
+  <si>
+    <t>productKey</t>
+  </si>
+  <si>
+    <t>Verify after product search, category and size dropdowns are displayed</t>
+  </si>
+  <si>
+    <t>Benadryl Itch Stopping Cream, Extra Strength, 1.3 Oz</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>expectedNewProduct</t>
+  </si>
+  <si>
+    <t>Verify correct product name is displayed after changing category and size for a product</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Chewable</t>
+    </r>
+  </si>
+  <si>
+    <t>60 count</t>
+  </si>
+  <si>
+    <t>Children's Benadryl Allergy Chewables, Grape, 3 Packs of 20 Count Each, 60 Count</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>storeName</t>
+  </si>
+  <si>
+    <t>expectedStoreUrl</t>
+  </si>
+  <si>
+    <t>Verify redirection to Amazon store</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Amazon.Com</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>Verify redirection to Walmart store</t>
+  </si>
+  <si>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/</t>
+  </si>
+  <si>
+    <t>Verify redirection to Target store</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>https://www.target.com/s?searchTerm=Benadryl</t>
+  </si>
+  <si>
+    <t>Verify redirection to CVS Pharmacy store</t>
+  </si>
+  <si>
+    <t>CVS Pharmacy</t>
+  </si>
+  <si>
+    <t>https://www.cvs.com/international.html</t>
+  </si>
+  <si>
+    <t>Verify redirection to Walgreens store</t>
+  </si>
+  <si>
+    <t>Walgreens</t>
+  </si>
+  <si>
+    <t>https://www.walgreens.com/search/results.jsp</t>
+  </si>
+  <si>
+    <t>Verify redirection to Rite Aid store</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Rite Aid</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.riteaid.com/?cjdata</t>
+  </si>
+  <si>
+    <t>Verify redirection to Family Dollar store</t>
+  </si>
+  <si>
+    <t>Family Dollar</t>
+  </si>
+  <si>
+    <t>https://www.familydollar.com/searchresults?Ntt=benadryl</t>
+  </si>
+  <si>
+    <t>Verify redirection to Dollar General store</t>
+  </si>
+  <si>
+    <t>Dollar General</t>
+  </si>
+  <si>
+    <t>https://www.dollargeneral.com/product-search.html?q=Benadryl</t>
+  </si>
+  <si>
+    <t>Verify relevant store locations are displayed on search using location</t>
   </si>
 </sst>
 </file>
@@ -50,7 +187,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +196,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -73,6 +218,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -203,12 +354,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -521,138 +678,143 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,7 +1136,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1012,4 +1174,369 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="65.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="13.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="48.1111111111111" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="32.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.amazon.com/"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.walmart.com/" tooltip="https://www.walmart.com/"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://www.target.com/s?searchTerm=Benadryl"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://www.cvs.com/international.html" tooltip="https://www.cvs.com/international.html"/>
+    <hyperlink ref="F9" r:id="rId5" display="https://www.dollargeneral.com/product-search.html?q=Benadryl"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>